<commit_message>
Tweaked F Model parameter file.
</commit_message>
<xml_diff>
--- a/Inputs/F_template_parameters_Model.xlsx
+++ b/Inputs/F_template_parameters_Model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/schlosser_paul_epa_gov/Documents/mcsim-5.6.5/PBPK_Model_Template_Mod/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="76" documentId="8_{7F8D94C6-EC2B-4A79-A22A-AD1B7807B962}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{88C5A103-251F-47FE-AE48-78D58A0E53D4}"/>
+  <xr:revisionPtr revIDLastSave="79" documentId="8_{7F8D94C6-EC2B-4A79-A22A-AD1B7807B962}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{30F759E8-85C1-4626-9B42-4EAF079863C5}"/>
   <bookViews>
-    <workbookView xWindow="2535" yWindow="795" windowWidth="21825" windowHeight="12915" xr2:uid="{089E7848-11EB-427A-89EA-83825F220BA0}"/>
+    <workbookView xWindow="-25515" yWindow="885" windowWidth="21825" windowHeight="12915" xr2:uid="{089E7848-11EB-427A-89EA-83825F220BA0}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameter_Set_1" sheetId="9" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="265">
   <si>
     <t>Code</t>
   </si>
@@ -827,7 +827,7 @@
     <t>bone</t>
   </si>
   <si>
-    <t>Jean et al. used 0.03 for adults</t>
+    <t>Jean et al. used 0.05 for children, 0.03 for adults</t>
   </si>
 </sst>
 </file>
@@ -971,6 +971,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1272,8 +1276,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ADCAA70-43B6-4F02-AE2A-67A6EACE5958}">
   <dimension ref="A1:J105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E97" sqref="E97"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I81" sqref="I81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1395,6 +1399,9 @@
       <c r="C8" t="s">
         <v>19</v>
       </c>
+      <c r="E8" t="s">
+        <v>182</v>
+      </c>
       <c r="F8" t="s">
         <v>241</v>
       </c>
@@ -2544,7 +2551,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>108</v>
       </c>
@@ -2561,7 +2568,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>109</v>
       </c>
@@ -2578,7 +2585,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>110</v>
       </c>
@@ -2595,7 +2602,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>111</v>
       </c>
@@ -2612,7 +2619,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>112</v>
       </c>
@@ -2635,8 +2642,10 @@
         <v>264</v>
       </c>
       <c r="H85" s="6"/>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I85" s="6"/>
+      <c r="J85" s="6"/>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>153</v>
       </c>
@@ -2661,7 +2670,7 @@
       </c>
       <c r="H86" s="5"/>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>121</v>
       </c>
@@ -2675,7 +2684,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>122</v>
       </c>
@@ -2689,7 +2698,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>123</v>
       </c>
@@ -2706,7 +2715,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>124</v>
       </c>
@@ -2723,7 +2732,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>125</v>
       </c>
@@ -2740,7 +2749,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>126</v>
       </c>
@@ -2754,7 +2763,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>127</v>
       </c>
@@ -2768,7 +2777,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>128</v>
       </c>
@@ -2782,7 +2791,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>129</v>
       </c>
@@ -2796,7 +2805,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>130</v>
       </c>
@@ -2933,48 +2942,8 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_Source xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
-    <Language xmlns="http://schemas.microsoft.com/sharepoint/v3">English</Language>
-    <j747ac98061d40f0aa7bd47e1db5675d xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </j747ac98061d40f0aa7bd47e1db5675d>
-    <External_x0020_Contributor xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <TaxKeywordTaxHTField xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </TaxKeywordTaxHTField>
-    <Record xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">Shared</Record>
-    <Rights xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <Document_x0020_Creation_x0020_Date xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">2020-10-14T20:30:29+00:00</Document_x0020_Creation_x0020_Date>
-    <EPA_x0020_Office xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <CategoryDescription xmlns="http://schemas.microsoft.com/sharepoint.v3" xsi:nil="true"/>
-    <Identifier xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <_Coverage xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
-    <Creator xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Creator>
-    <EPA_x0020_Related_x0020_Documents xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <EPA_x0020_Contributor xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </EPA_x0020_Contributor>
-    <TaxCatchAll xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <e3f09c3df709400db2417a7161762d62 xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </e3f09c3df709400db2417a7161762d62>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="2ba80736-48fa-4d73-aaff-bacaeeed013a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="29f62856-1543-49d4-a736-4569d363f533" ContentTypeId="0x0101" PreviousValue="false"/>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3451,8 +3420,48 @@
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="29f62856-1543-49d4-a736-4569d363f533" ContentTypeId="0x0101" PreviousValue="false"/>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_Source xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
+    <Language xmlns="http://schemas.microsoft.com/sharepoint/v3">English</Language>
+    <j747ac98061d40f0aa7bd47e1db5675d xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </j747ac98061d40f0aa7bd47e1db5675d>
+    <External_x0020_Contributor xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <TaxKeywordTaxHTField xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </TaxKeywordTaxHTField>
+    <Record xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">Shared</Record>
+    <Rights xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <Document_x0020_Creation_x0020_Date xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">2020-10-14T20:30:29+00:00</Document_x0020_Creation_x0020_Date>
+    <EPA_x0020_Office xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <CategoryDescription xmlns="http://schemas.microsoft.com/sharepoint.v3" xsi:nil="true"/>
+    <Identifier xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <_Coverage xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
+    <Creator xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Creator>
+    <EPA_x0020_Related_x0020_Documents xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <EPA_x0020_Contributor xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </EPA_x0020_Contributor>
+    <TaxCatchAll xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <e3f09c3df709400db2417a7161762d62 xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </e3f09c3df709400db2417a7161762d62>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="2ba80736-48fa-4d73-aaff-bacaeeed013a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3464,16 +3473,9 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA939294-F21F-45CD-81A6-3A616888DAC5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C4A2D8C-C5B5-46A0-8FC1-3730CC1A83D7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4"/>
-    <ds:schemaRef ds:uri="93237db7-bebb-43bb-9414-bc3313990c09"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint.v3"/>
-    <ds:schemaRef ds:uri="2ba80736-48fa-4d73-aaff-bacaeeed013a"/>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3502,9 +3504,16 @@
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C4A2D8C-C5B5-46A0-8FC1-3730CC1A83D7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA939294-F21F-45CD-81A6-3A616888DAC5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4"/>
+    <ds:schemaRef ds:uri="93237db7-bebb-43bb-9414-bc3313990c09"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint.v3"/>
+    <ds:schemaRef ds:uri="2ba80736-48fa-4d73-aaff-bacaeeed013a"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>